<commit_message>
[New] Visualization of building blocks in html file
</commit_message>
<xml_diff>
--- a/output/test-nodes.xlsx
+++ b/output/test-nodes.xlsx
@@ -55,7 +55,7 @@
     <t>elections</t>
   </si>
   <si>
-    <t>country 's elections, elections, recent elections, many elections</t>
+    <t>country 's elections, many elections, elections, recent elections</t>
   </si>
   <si>
     <t>part</t>
@@ -73,7 +73,7 @@
     <t>technology</t>
   </si>
   <si>
-    <t>actual technology, this new technology</t>
+    <t>this new technology, actual technology</t>
   </si>
   <si>
     <t>worries</t>
@@ -226,7 +226,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>other common type, this type</t>
+    <t>this type, other common type</t>
   </si>
   <si>
     <t>world</t>

</xml_diff>

<commit_message>
[New] One more rule for today
</commit_message>
<xml_diff>
--- a/output/test-nodes.xlsx
+++ b/output/test-nodes.xlsx
@@ -25,7 +25,7 @@
     <t>ink</t>
   </si>
   <si>
-    <t>indelible visible ink, ink</t>
+    <t>ink, indelible visible ink</t>
   </si>
   <si>
     <t>democracy</t>
@@ -55,7 +55,7 @@
     <t>elections</t>
   </si>
   <si>
-    <t>upcoming parliamentary elections, these elections, recent elections, many elections, elections, country 's elections</t>
+    <t>country 's elections, recent elections, many elections, these elections, elections, upcoming parliamentary elections</t>
   </si>
   <si>
     <t>part</t>
@@ -64,7 +64,7 @@
     <t>drive</t>
   </si>
   <si>
-    <t>petition drive, drive</t>
+    <t>drive, petition drive</t>
   </si>
   <si>
     <t>island</t>
@@ -79,7 +79,7 @@
     <t>use</t>
   </si>
   <si>
-    <t>improper use, use</t>
+    <t>use, improper use</t>
   </si>
   <si>
     <t>parliamentary</t>

</xml_diff>